<commit_message>
FastKey Version 2.0.0 release
</commit_message>
<xml_diff>
--- a/doku/Shortcuts.xlsx
+++ b/doku/Shortcuts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e561a338f4e23b8e/Dokumente/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucak\SynologyDrive\GithubRepos\fastKey\doku\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1320" documentId="8_{0ECA89DE-96A3-4B6A-AE58-465BAE8B3EB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A13036A3-BAF5-459E-BC03-2FFD2A76FCD3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9451733C-DAD5-482B-AD0E-B54244E08D31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{60267EAC-A2D4-4046-96D4-097EDA30F2D3}"/>
+    <workbookView xWindow="1485" yWindow="240" windowWidth="49650" windowHeight="21015" xr2:uid="{60267EAC-A2D4-4046-96D4-097EDA30F2D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle2" sheetId="2" r:id="rId1"/>
@@ -546,9 +546,6 @@
     <t>markdown.preview.refresh</t>
   </si>
   <si>
-    <t>strg + k | r</t>
-  </si>
-  <si>
     <t>refresh markdown</t>
   </si>
   <si>
@@ -612,9 +609,6 @@
     <t>strg + k |c</t>
   </si>
   <si>
-    <t>strg + k | strg + f</t>
-  </si>
-  <si>
     <t>add folder to workspace</t>
   </si>
   <si>
@@ -642,9 +636,6 @@
     <t xml:space="preserve">strg + ´ </t>
   </si>
   <si>
-    <t>strg + shift + `</t>
-  </si>
-  <si>
     <t>Tab Control</t>
   </si>
   <si>
@@ -658,9 +649,6 @@
   </si>
   <si>
     <t>create new file</t>
-  </si>
-  <si>
-    <t>strg + shift + o</t>
   </si>
   <si>
     <t>close current tab</t>
@@ -1245,6 +1233,18 @@
   </si>
   <si>
     <t>workbench.action.quickOpen</t>
+  </si>
+  <si>
+    <t>strg + k | a</t>
+  </si>
+  <si>
+    <t>strg + k | l</t>
+  </si>
+  <si>
+    <t>strg + alt + o</t>
+  </si>
+  <si>
+    <t>strg + alt + `</t>
   </si>
 </sst>
 </file>
@@ -1711,20 +1711,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DC1306C-28AC-4BD7-AF93-2979151AEB79}">
   <dimension ref="A1:AJ119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G68" sqref="G68"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O80" sqref="O80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="8" width="31.5546875" customWidth="1"/>
-    <col min="9" max="9" width="67.109375" customWidth="1"/>
-    <col min="14" max="14" width="43.5546875" customWidth="1"/>
-    <col min="15" max="15" width="38.88671875" customWidth="1"/>
-    <col min="16" max="16" width="67.109375" customWidth="1"/>
+    <col min="7" max="8" width="31.5703125" customWidth="1"/>
+    <col min="9" max="9" width="67.140625" customWidth="1"/>
+    <col min="14" max="14" width="43.5703125" customWidth="1"/>
+    <col min="15" max="15" width="38.85546875" customWidth="1"/>
+    <col min="16" max="16" width="67.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="8"/>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -1762,7 +1762,7 @@
       <c r="AI1" s="8"/>
       <c r="AJ1" s="8"/>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -1800,7 +1800,7 @@
       <c r="AI2" s="8"/>
       <c r="AJ2" s="8"/>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
@@ -1838,7 +1838,7 @@
       <c r="AI3" s="8"/>
       <c r="AJ3" s="8"/>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -1876,7 +1876,7 @@
       <c r="AI4" s="8"/>
       <c r="AJ4" s="8"/>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -1914,7 +1914,7 @@
       <c r="AI5" s="8"/>
       <c r="AJ5" s="8"/>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
@@ -1952,7 +1952,7 @@
       <c r="AI6" s="8"/>
       <c r="AJ6" s="8"/>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -1990,7 +1990,7 @@
       <c r="AI7" s="8"/>
       <c r="AJ7" s="8"/>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -2028,7 +2028,7 @@
       <c r="AI8" s="8"/>
       <c r="AJ8" s="8"/>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -2066,7 +2066,7 @@
       <c r="AI9" s="8"/>
       <c r="AJ9" s="8"/>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -2104,7 +2104,7 @@
       <c r="AI10" s="8"/>
       <c r="AJ10" s="8"/>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -2142,7 +2142,7 @@
       <c r="AI11" s="8"/>
       <c r="AJ11" s="8"/>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -2180,7 +2180,7 @@
       <c r="AI12" s="8"/>
       <c r="AJ12" s="8"/>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -2218,7 +2218,7 @@
       <c r="AI13" s="8"/>
       <c r="AJ13" s="8"/>
     </row>
-    <row r="14" spans="1:36" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:36" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -2226,7 +2226,7 @@
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
       <c r="G14" s="17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H14" s="17"/>
       <c r="I14" s="17"/>
@@ -2235,7 +2235,7 @@
       <c r="L14" s="8"/>
       <c r="M14" s="8"/>
       <c r="N14" s="17" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="O14" s="17"/>
       <c r="P14" s="17"/>
@@ -2260,7 +2260,7 @@
       <c r="AI14" s="8"/>
       <c r="AJ14" s="8"/>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
@@ -2298,7 +2298,7 @@
       <c r="AI15" s="8"/>
       <c r="AJ15" s="8"/>
     </row>
-    <row r="16" spans="1:36" ht="18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:36" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -2348,7 +2348,7 @@
       <c r="AI16" s="8"/>
       <c r="AJ16" s="8"/>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -2369,10 +2369,10 @@
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
       <c r="N17" s="3" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="O17" s="13" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="P17" s="12" t="s">
         <v>67</v>
@@ -2398,7 +2398,7 @@
       <c r="AI17" s="8"/>
       <c r="AJ17" s="8"/>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
@@ -2419,7 +2419,7 @@
       <c r="L18" s="8"/>
       <c r="M18" s="8"/>
       <c r="N18" s="3" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="O18" s="1" t="s">
         <v>66</v>
@@ -2448,7 +2448,7 @@
       <c r="AI18" s="8"/>
       <c r="AJ18" s="8"/>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -2469,10 +2469,10 @@
       <c r="L19" s="8"/>
       <c r="M19" s="8"/>
       <c r="N19" s="14" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="O19" s="15" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="P19" s="16" t="s">
         <v>69</v>
@@ -2498,7 +2498,7 @@
       <c r="AI19" s="8"/>
       <c r="AJ19" s="8"/>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -2509,7 +2509,7 @@
         <v>85</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="I20" s="12" t="s">
         <v>84</v>
@@ -2519,10 +2519,10 @@
       <c r="L20" s="8"/>
       <c r="M20" s="8"/>
       <c r="N20" s="3" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="P20" s="12" t="s">
         <v>125</v>
@@ -2548,7 +2548,7 @@
       <c r="AI20" s="8"/>
       <c r="AJ20" s="8"/>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
@@ -2559,7 +2559,7 @@
         <v>86</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="I21" s="12" t="s">
         <v>87</v>
@@ -2569,13 +2569,13 @@
       <c r="L21" s="8"/>
       <c r="M21" s="8"/>
       <c r="N21" s="3" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="P21" s="12" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="Q21" s="8"/>
       <c r="R21" s="8"/>
@@ -2598,7 +2598,7 @@
       <c r="AI21" s="8"/>
       <c r="AJ21" s="8"/>
     </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
@@ -2619,10 +2619,10 @@
       <c r="L22" s="8"/>
       <c r="M22" s="8"/>
       <c r="N22" s="3" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="P22" s="12" t="s">
         <v>123</v>
@@ -2648,7 +2648,7 @@
       <c r="AI22" s="8"/>
       <c r="AJ22" s="8"/>
     </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
@@ -2669,10 +2669,10 @@
       <c r="L23" s="8"/>
       <c r="M23" s="8"/>
       <c r="N23" s="3" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="P23" s="12" t="s">
         <v>124</v>
@@ -2698,7 +2698,7 @@
       <c r="AI23" s="8"/>
       <c r="AJ23" s="8"/>
     </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -2709,7 +2709,7 @@
         <v>88</v>
       </c>
       <c r="H24" s="13" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="I24" s="12" t="s">
         <v>99</v>
@@ -2719,13 +2719,13 @@
       <c r="L24" s="8"/>
       <c r="M24" s="8"/>
       <c r="N24" s="3" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="P24" s="12" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="Q24" s="8"/>
       <c r="R24" s="8"/>
@@ -2748,7 +2748,7 @@
       <c r="AI24" s="8"/>
       <c r="AJ24" s="8"/>
     </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
@@ -2759,7 +2759,7 @@
         <v>89</v>
       </c>
       <c r="H25" s="13" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="I25" s="12" t="s">
         <v>101</v>
@@ -2769,13 +2769,13 @@
       <c r="L25" s="8"/>
       <c r="M25" s="8"/>
       <c r="N25" s="3" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="O25" s="1" t="s">
         <v>61</v>
       </c>
       <c r="P25" s="12" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="Q25" s="8"/>
       <c r="R25" s="8"/>
@@ -2798,7 +2798,7 @@
       <c r="AI25" s="8"/>
       <c r="AJ25" s="8"/>
     </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
@@ -2809,7 +2809,7 @@
         <v>90</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="I26" s="12" t="s">
         <v>100</v>
@@ -2819,13 +2819,13 @@
       <c r="L26" s="8"/>
       <c r="M26" s="8"/>
       <c r="N26" s="3" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="O26" s="1" t="s">
         <v>155</v>
       </c>
       <c r="P26" s="12" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="Q26" s="8"/>
       <c r="R26" s="8"/>
@@ -2848,7 +2848,7 @@
       <c r="AI26" s="8"/>
       <c r="AJ26" s="8"/>
     </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
@@ -2859,7 +2859,7 @@
         <v>91</v>
       </c>
       <c r="H27" s="13" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="I27" s="12" t="s">
         <v>98</v>
@@ -2869,13 +2869,13 @@
       <c r="L27" s="8"/>
       <c r="M27" s="8"/>
       <c r="N27" s="3" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="O27" s="1" t="s">
         <v>61</v>
       </c>
       <c r="P27" s="12" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="Q27" s="8"/>
       <c r="R27" s="8"/>
@@ -2898,20 +2898,20 @@
       <c r="AI27" s="8"/>
       <c r="AJ27" s="8"/>
     </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
       <c r="F28" s="8" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>92</v>
       </c>
       <c r="H28" s="13" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="I28" s="12" t="s">
         <v>97</v>
@@ -2921,13 +2921,13 @@
       <c r="L28" s="8"/>
       <c r="M28" s="8"/>
       <c r="N28" s="3" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="P28" s="12" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="Q28" s="8"/>
       <c r="R28" s="8"/>
@@ -2950,7 +2950,7 @@
       <c r="AI28" s="8"/>
       <c r="AJ28" s="8"/>
     </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
@@ -2961,7 +2961,7 @@
         <v>93</v>
       </c>
       <c r="H29" s="13" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="I29" s="12" t="s">
         <v>96</v>
@@ -2971,13 +2971,13 @@
       <c r="L29" s="8"/>
       <c r="M29" s="8"/>
       <c r="N29" s="3" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="P29" s="12" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="Q29" s="8"/>
       <c r="R29" s="8"/>
@@ -3000,7 +3000,7 @@
       <c r="AI29" s="8"/>
       <c r="AJ29" s="8"/>
     </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
@@ -3011,7 +3011,7 @@
         <v>94</v>
       </c>
       <c r="H30" s="13" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="I30" s="12" t="s">
         <v>95</v>
@@ -3021,10 +3021,10 @@
       <c r="L30" s="8"/>
       <c r="M30" s="8"/>
       <c r="N30" s="3" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="P30" s="12" t="s">
         <v>60</v>
@@ -3050,7 +3050,7 @@
       <c r="AI30" s="8"/>
       <c r="AJ30" s="8"/>
     </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
@@ -3061,7 +3061,7 @@
         <v>137</v>
       </c>
       <c r="H31" s="13" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="I31" s="12" t="s">
         <v>136</v>
@@ -3071,10 +3071,10 @@
       <c r="L31" s="8"/>
       <c r="M31" s="8"/>
       <c r="N31" s="3" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="P31" s="12" t="s">
         <v>62</v>
@@ -3100,7 +3100,7 @@
       <c r="AI31" s="8"/>
       <c r="AJ31" s="8"/>
     </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
@@ -3111,7 +3111,7 @@
         <v>157</v>
       </c>
       <c r="H32" s="13" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="I32" s="12" t="s">
         <v>156</v>
@@ -3121,10 +3121,10 @@
       <c r="L32" s="8"/>
       <c r="M32" s="8"/>
       <c r="N32" s="3" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="P32" s="12" t="s">
         <v>58</v>
@@ -3150,7 +3150,7 @@
       <c r="AI32" s="8"/>
       <c r="AJ32" s="8"/>
     </row>
-    <row r="33" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
@@ -3161,7 +3161,7 @@
         <v>159</v>
       </c>
       <c r="H33" s="13" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="I33" s="12" t="s">
         <v>158</v>
@@ -3171,10 +3171,10 @@
       <c r="L33" s="8"/>
       <c r="M33" s="8"/>
       <c r="N33" s="3" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="P33" s="12" t="s">
         <v>53</v>
@@ -3200,7 +3200,7 @@
       <c r="AI33" s="8"/>
       <c r="AJ33" s="8"/>
     </row>
-    <row r="34" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
@@ -3211,7 +3211,7 @@
         <v>140</v>
       </c>
       <c r="H34" s="13" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="I34" s="12" t="s">
         <v>139</v>
@@ -3224,7 +3224,7 @@
         <v>127</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="P34" s="12" t="s">
         <v>126</v>
@@ -3250,7 +3250,7 @@
       <c r="AI34" s="8"/>
       <c r="AJ34" s="8"/>
     </row>
-    <row r="35" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
@@ -3258,10 +3258,10 @@
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
       <c r="G35" s="3" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="H35" s="13" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="I35" s="12" t="s">
         <v>59</v>
@@ -3274,7 +3274,7 @@
         <v>127</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="P35" s="12" t="s">
         <v>128</v>
@@ -3300,7 +3300,7 @@
       <c r="AI35" s="8"/>
       <c r="AJ35" s="8"/>
     </row>
-    <row r="36" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
@@ -3324,7 +3324,7 @@
         <v>132</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="P36" s="12" t="s">
         <v>129</v>
@@ -3350,7 +3350,7 @@
       <c r="AI36" s="8"/>
       <c r="AJ36" s="8"/>
     </row>
-    <row r="37" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
@@ -3374,7 +3374,7 @@
         <v>131</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="P37" s="12" t="s">
         <v>130</v>
@@ -3400,7 +3400,7 @@
       <c r="AI37" s="8"/>
       <c r="AJ37" s="8"/>
     </row>
-    <row r="38" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
@@ -3421,13 +3421,13 @@
       <c r="L38" s="8"/>
       <c r="M38" s="8"/>
       <c r="N38" s="3" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="P38" s="12" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="Q38" s="8"/>
       <c r="R38" s="8"/>
@@ -3450,7 +3450,7 @@
       <c r="AI38" s="8"/>
       <c r="AJ38" s="8"/>
     </row>
-    <row r="39" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
@@ -3458,10 +3458,10 @@
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
       <c r="G39" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="H39" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>172</v>
       </c>
       <c r="I39" s="12" t="s">
         <v>169</v>
@@ -3494,7 +3494,7 @@
       <c r="AI39" s="8"/>
       <c r="AJ39" s="8"/>
     </row>
-    <row r="40" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
@@ -3502,13 +3502,13 @@
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
       <c r="G40" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I40" s="12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J40" s="8"/>
       <c r="K40" s="8"/>
@@ -3538,7 +3538,7 @@
       <c r="AI40" s="8"/>
       <c r="AJ40" s="8"/>
     </row>
-    <row r="41" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
@@ -3546,13 +3546,13 @@
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
       <c r="G41" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="I41" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J41" s="8"/>
       <c r="K41" s="8"/>
@@ -3582,7 +3582,7 @@
       <c r="AI41" s="8"/>
       <c r="AJ41" s="8"/>
     </row>
-    <row r="42" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A42" s="8"/>
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>
@@ -3590,13 +3590,13 @@
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
       <c r="G42" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="I42" s="12" t="s">
         <v>179</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="I42" s="12" t="s">
-        <v>180</v>
       </c>
       <c r="J42" s="8"/>
       <c r="K42" s="8"/>
@@ -3626,7 +3626,7 @@
       <c r="AI42" s="8"/>
       <c r="AJ42" s="8"/>
     </row>
-    <row r="43" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
@@ -3634,13 +3634,13 @@
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>
       <c r="G43" s="3" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="I43" s="12" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="J43" s="8"/>
       <c r="K43" s="8"/>
@@ -3670,7 +3670,7 @@
       <c r="AI43" s="8"/>
       <c r="AJ43" s="8"/>
     </row>
-    <row r="44" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
       <c r="B44" s="8"/>
       <c r="C44" s="8"/>
@@ -3708,7 +3708,7 @@
       <c r="AI44" s="8"/>
       <c r="AJ44" s="8"/>
     </row>
-    <row r="45" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A45" s="8"/>
       <c r="B45" s="8"/>
       <c r="C45" s="8"/>
@@ -3746,7 +3746,7 @@
       <c r="AI45" s="8"/>
       <c r="AJ45" s="8"/>
     </row>
-    <row r="46" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A46" s="8"/>
       <c r="B46" s="8"/>
       <c r="C46" s="8"/>
@@ -3784,7 +3784,7 @@
       <c r="AI46" s="8"/>
       <c r="AJ46" s="8"/>
     </row>
-    <row r="47" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A47" s="8"/>
       <c r="B47" s="8"/>
       <c r="C47" s="8"/>
@@ -3822,7 +3822,7 @@
       <c r="AI47" s="8"/>
       <c r="AJ47" s="8"/>
     </row>
-    <row r="48" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A48" s="8"/>
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
@@ -3860,7 +3860,7 @@
       <c r="AI48" s="8"/>
       <c r="AJ48" s="8"/>
     </row>
-    <row r="49" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A49" s="8"/>
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
@@ -3898,7 +3898,7 @@
       <c r="AI49" s="8"/>
       <c r="AJ49" s="8"/>
     </row>
-    <row r="50" spans="1:36" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:36" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="8"/>
       <c r="B50" s="8"/>
       <c r="C50" s="8"/>
@@ -3906,7 +3906,7 @@
       <c r="E50" s="8"/>
       <c r="F50" s="8"/>
       <c r="G50" s="17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H50" s="17"/>
       <c r="I50" s="17"/>
@@ -3915,7 +3915,7 @@
       <c r="L50" s="8"/>
       <c r="M50" s="8"/>
       <c r="N50" s="17" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="O50" s="17"/>
       <c r="P50" s="17"/>
@@ -3940,7 +3940,7 @@
       <c r="AI50" s="8"/>
       <c r="AJ50" s="8"/>
     </row>
-    <row r="51" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A51" s="8"/>
       <c r="B51" s="8"/>
       <c r="C51" s="8"/>
@@ -3978,7 +3978,7 @@
       <c r="AI51" s="8"/>
       <c r="AJ51" s="8"/>
     </row>
-    <row r="52" spans="1:36" ht="18" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:36" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A52" s="8"/>
       <c r="B52" s="8"/>
       <c r="C52" s="8"/>
@@ -4028,7 +4028,7 @@
       <c r="AI52" s="8"/>
       <c r="AJ52" s="8"/>
     </row>
-    <row r="53" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A53" s="8"/>
       <c r="B53" s="8"/>
       <c r="C53" s="8"/>
@@ -4036,7 +4036,7 @@
       <c r="E53" s="8"/>
       <c r="F53" s="8"/>
       <c r="G53" s="3" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="H53" s="1" t="s">
         <v>70</v>
@@ -4049,7 +4049,7 @@
       <c r="L53" s="8"/>
       <c r="M53" s="8"/>
       <c r="N53" s="3" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="O53" s="1" t="s">
         <v>4</v>
@@ -4078,7 +4078,7 @@
       <c r="AI53" s="8"/>
       <c r="AJ53" s="8"/>
     </row>
-    <row r="54" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A54" s="8"/>
       <c r="B54" s="8"/>
       <c r="C54" s="8"/>
@@ -4086,13 +4086,13 @@
       <c r="E54" s="8"/>
       <c r="F54" s="8"/>
       <c r="G54" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="I54" s="12" t="s">
         <v>183</v>
-      </c>
-      <c r="H54" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="I54" s="12" t="s">
-        <v>184</v>
       </c>
       <c r="J54" s="8"/>
       <c r="K54" s="8"/>
@@ -4128,7 +4128,7 @@
       <c r="AI54" s="8"/>
       <c r="AJ54" s="8"/>
     </row>
-    <row r="55" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A55" s="8"/>
       <c r="B55" s="8"/>
       <c r="C55" s="8"/>
@@ -4136,10 +4136,10 @@
       <c r="E55" s="8"/>
       <c r="F55" s="8"/>
       <c r="G55" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="H55" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="H55" s="1" t="s">
-        <v>186</v>
       </c>
       <c r="I55" s="12" t="s">
         <v>134</v>
@@ -4149,7 +4149,7 @@
       <c r="L55" s="8"/>
       <c r="M55" s="8"/>
       <c r="N55" s="3" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="O55" s="1" t="s">
         <v>10</v>
@@ -4178,7 +4178,7 @@
       <c r="AI55" s="8"/>
       <c r="AJ55" s="8"/>
     </row>
-    <row r="56" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A56" s="8"/>
       <c r="B56" s="8"/>
       <c r="C56" s="8"/>
@@ -4186,10 +4186,10 @@
       <c r="E56" s="8"/>
       <c r="F56" s="8"/>
       <c r="G56" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I56" s="12" t="s">
         <v>133</v>
@@ -4228,7 +4228,7 @@
       <c r="AI56" s="8"/>
       <c r="AJ56" s="8"/>
     </row>
-    <row r="57" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A57" s="8"/>
       <c r="B57" s="8"/>
       <c r="C57" s="8"/>
@@ -4236,10 +4236,10 @@
       <c r="E57" s="8"/>
       <c r="F57" s="8"/>
       <c r="G57" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I57" s="12" t="s">
         <v>135</v>
@@ -4249,13 +4249,13 @@
       <c r="L57" s="8"/>
       <c r="M57" s="8"/>
       <c r="N57" s="3" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="O57" s="1" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="P57" s="12" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="Q57" s="8"/>
       <c r="R57" s="8"/>
@@ -4278,7 +4278,7 @@
       <c r="AI57" s="8"/>
       <c r="AJ57" s="8"/>
     </row>
-    <row r="58" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A58" s="8"/>
       <c r="B58" s="8"/>
       <c r="C58" s="8"/>
@@ -4286,26 +4286,26 @@
       <c r="E58" s="8"/>
       <c r="F58" s="8"/>
       <c r="G58" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>192</v>
+        <v>387</v>
       </c>
       <c r="I58" s="12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J58" s="8"/>
       <c r="K58" s="8"/>
       <c r="L58" s="8"/>
       <c r="M58" s="8"/>
       <c r="N58" s="3" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="O58" s="1" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="P58" s="12" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="Q58" s="8"/>
       <c r="R58" s="8"/>
@@ -4328,7 +4328,7 @@
       <c r="AI58" s="8"/>
       <c r="AJ58" s="8"/>
     </row>
-    <row r="59" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A59" s="8"/>
       <c r="B59" s="8"/>
       <c r="C59" s="8"/>
@@ -4336,26 +4336,26 @@
       <c r="E59" s="8"/>
       <c r="F59" s="8"/>
       <c r="G59" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>170</v>
+        <v>388</v>
       </c>
       <c r="I59" s="12" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="J59" s="8"/>
       <c r="K59" s="8"/>
       <c r="L59" s="8"/>
       <c r="M59" s="8"/>
       <c r="N59" s="3" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="O59" s="1" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="P59" s="12" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="Q59" s="8"/>
       <c r="R59" s="8"/>
@@ -4378,7 +4378,7 @@
       <c r="AI59" s="8"/>
       <c r="AJ59" s="8"/>
     </row>
-    <row r="60" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A60" s="8"/>
       <c r="B60" s="8"/>
       <c r="C60" s="8"/>
@@ -4386,26 +4386,26 @@
       <c r="E60" s="8"/>
       <c r="F60" s="8"/>
       <c r="G60" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="I60" s="12" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J60" s="8"/>
       <c r="K60" s="8"/>
       <c r="L60" s="8"/>
       <c r="M60" s="8"/>
       <c r="N60" s="3" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="O60" s="1" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="P60" s="12" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="Q60" s="8"/>
       <c r="R60" s="8"/>
@@ -4428,7 +4428,7 @@
       <c r="AI60" s="8"/>
       <c r="AJ60" s="8"/>
     </row>
-    <row r="61" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A61" s="8"/>
       <c r="B61" s="8"/>
       <c r="C61" s="8"/>
@@ -4436,10 +4436,10 @@
       <c r="E61" s="8"/>
       <c r="F61" s="8"/>
       <c r="G61" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="H61" s="1" t="s">
         <v>199</v>
-      </c>
-      <c r="H61" s="1" t="s">
-        <v>201</v>
       </c>
       <c r="I61" s="12" t="s">
         <v>63</v>
@@ -4478,7 +4478,7 @@
       <c r="AI61" s="8"/>
       <c r="AJ61" s="8"/>
     </row>
-    <row r="62" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A62" s="8"/>
       <c r="B62" s="8"/>
       <c r="C62" s="8"/>
@@ -4486,10 +4486,10 @@
       <c r="E62" s="8"/>
       <c r="F62" s="8"/>
       <c r="G62" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>202</v>
+        <v>390</v>
       </c>
       <c r="I62" s="12" t="s">
         <v>64</v>
@@ -4502,7 +4502,7 @@
         <v>19</v>
       </c>
       <c r="O62" s="1" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="P62" s="12" t="s">
         <v>20</v>
@@ -4528,7 +4528,7 @@
       <c r="AI62" s="8"/>
       <c r="AJ62" s="8"/>
     </row>
-    <row r="63" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A63" s="8"/>
       <c r="B63" s="8"/>
       <c r="C63" s="8"/>
@@ -4542,7 +4542,7 @@
         <v>75</v>
       </c>
       <c r="I63" s="12" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="J63" s="8"/>
       <c r="K63" s="8"/>
@@ -4552,7 +4552,7 @@
         <v>21</v>
       </c>
       <c r="O63" s="1" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="P63" s="12" t="s">
         <v>22</v>
@@ -4578,7 +4578,7 @@
       <c r="AI63" s="8"/>
       <c r="AJ63" s="8"/>
     </row>
-    <row r="64" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A64" s="8"/>
       <c r="B64" s="8"/>
       <c r="C64" s="8"/>
@@ -4589,7 +4589,7 @@
         <v>78</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="I64" s="12" t="s">
         <v>77</v>
@@ -4602,7 +4602,7 @@
         <v>23</v>
       </c>
       <c r="O64" s="1" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="P64" s="12" t="s">
         <v>24</v>
@@ -4628,7 +4628,7 @@
       <c r="AI64" s="8"/>
       <c r="AJ64" s="8"/>
     </row>
-    <row r="65" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A65" s="8"/>
       <c r="B65" s="8"/>
       <c r="C65" s="8"/>
@@ -4636,7 +4636,7 @@
       <c r="E65" s="8"/>
       <c r="F65" s="8"/>
       <c r="G65" s="3" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="H65" s="1" t="s">
         <v>80</v>
@@ -4649,7 +4649,7 @@
       <c r="L65" s="8"/>
       <c r="M65" s="8"/>
       <c r="N65" s="3" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="O65" s="1" t="s">
         <v>25</v>
@@ -4678,7 +4678,7 @@
       <c r="AI65" s="8"/>
       <c r="AJ65" s="8"/>
     </row>
-    <row r="66" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A66" s="8"/>
       <c r="B66" s="8"/>
       <c r="C66" s="8"/>
@@ -4702,10 +4702,10 @@
         <v>27</v>
       </c>
       <c r="O66" s="1" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="P66" s="12" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="Q66" s="8"/>
       <c r="R66" s="8"/>
@@ -4728,7 +4728,7 @@
       <c r="AI66" s="8"/>
       <c r="AJ66" s="8"/>
     </row>
-    <row r="67" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A67" s="8"/>
       <c r="B67" s="8"/>
       <c r="C67" s="8"/>
@@ -4736,23 +4736,23 @@
       <c r="E67" s="8"/>
       <c r="F67" s="8"/>
       <c r="G67" s="3" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="I67" s="12" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="J67" s="8"/>
       <c r="K67" s="8"/>
       <c r="L67" s="8"/>
       <c r="M67" s="8"/>
       <c r="N67" s="3" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="O67" s="1" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="P67" s="12" t="s">
         <v>29</v>
@@ -4778,7 +4778,7 @@
       <c r="AI67" s="8"/>
       <c r="AJ67" s="8"/>
     </row>
-    <row r="68" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A68" s="8"/>
       <c r="B68" s="8"/>
       <c r="C68" s="8"/>
@@ -4786,10 +4786,10 @@
       <c r="E68" s="8"/>
       <c r="F68" s="8"/>
       <c r="G68" s="3" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="I68" s="12" t="s">
         <v>58</v>
@@ -4799,10 +4799,10 @@
       <c r="L68" s="8"/>
       <c r="M68" s="8"/>
       <c r="N68" s="3" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="O68" s="1" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="P68" s="12" t="s">
         <v>41</v>
@@ -4828,7 +4828,7 @@
       <c r="AI68" s="8"/>
       <c r="AJ68" s="8"/>
     </row>
-    <row r="69" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A69" s="8"/>
       <c r="B69" s="8"/>
       <c r="C69" s="8"/>
@@ -4846,7 +4846,7 @@
         <v>42</v>
       </c>
       <c r="O69" s="1" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="P69" s="12" t="s">
         <v>40</v>
@@ -4869,7 +4869,7 @@
       <c r="AF69" s="8"/>
       <c r="AG69" s="8"/>
     </row>
-    <row r="70" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A70" s="8"/>
       <c r="B70" s="8"/>
       <c r="C70" s="8"/>
@@ -4884,10 +4884,10 @@
       <c r="L70" s="8"/>
       <c r="M70" s="8"/>
       <c r="N70" s="3" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="O70" s="1" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="P70" s="12" t="s">
         <v>39</v>
@@ -4910,7 +4910,7 @@
       <c r="AF70" s="8"/>
       <c r="AG70" s="8"/>
     </row>
-    <row r="71" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A71" s="8"/>
       <c r="B71" s="8"/>
       <c r="C71" s="8"/>
@@ -4925,7 +4925,7 @@
       <c r="L71" s="8"/>
       <c r="M71" s="8"/>
       <c r="N71" s="3" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="O71" s="1" t="s">
         <v>68</v>
@@ -4951,7 +4951,7 @@
       <c r="AF71" s="8"/>
       <c r="AG71" s="8"/>
     </row>
-    <row r="72" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A72" s="8"/>
       <c r="B72" s="8"/>
       <c r="C72" s="8"/>
@@ -4966,10 +4966,10 @@
       <c r="L72" s="8"/>
       <c r="M72" s="8"/>
       <c r="N72" s="3" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="O72" s="1" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="P72" s="12" t="s">
         <v>36</v>
@@ -4992,7 +4992,7 @@
       <c r="AF72" s="8"/>
       <c r="AG72" s="8"/>
     </row>
-    <row r="73" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A73" s="8"/>
       <c r="B73" s="8"/>
       <c r="C73" s="8"/>
@@ -5007,10 +5007,10 @@
       <c r="L73" s="8"/>
       <c r="M73" s="8"/>
       <c r="N73" s="3" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="O73" s="1" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="P73" s="12" t="s">
         <v>37</v>
@@ -5033,7 +5033,7 @@
       <c r="AF73" s="8"/>
       <c r="AG73" s="8"/>
     </row>
-    <row r="74" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A74" s="8"/>
       <c r="B74" s="8"/>
       <c r="C74" s="8"/>
@@ -5074,7 +5074,7 @@
       <c r="AF74" s="8"/>
       <c r="AG74" s="8"/>
     </row>
-    <row r="75" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A75" s="8"/>
       <c r="B75" s="8"/>
       <c r="C75" s="8"/>
@@ -5092,7 +5092,7 @@
         <v>45</v>
       </c>
       <c r="O75" s="1" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="P75" s="12" t="s">
         <v>46</v>
@@ -5115,7 +5115,7 @@
       <c r="AF75" s="8"/>
       <c r="AG75" s="8"/>
     </row>
-    <row r="76" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A76" s="8"/>
       <c r="B76" s="8"/>
       <c r="C76" s="8"/>
@@ -5133,7 +5133,7 @@
         <v>115</v>
       </c>
       <c r="O76" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="P76" s="12" t="s">
         <v>116</v>
@@ -5156,7 +5156,7 @@
       <c r="AF76" s="8"/>
       <c r="AG76" s="8"/>
     </row>
-    <row r="77" spans="1:36" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:36" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A77" s="8"/>
       <c r="B77" s="8"/>
       <c r="C77" s="8"/>
@@ -5164,7 +5164,7 @@
       <c r="E77" s="8"/>
       <c r="F77" s="8"/>
       <c r="G77" s="17" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="H77" s="17"/>
       <c r="I77" s="17"/>
@@ -5176,7 +5176,7 @@
         <v>117</v>
       </c>
       <c r="O77" s="1" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="P77" s="12" t="s">
         <v>118</v>
@@ -5199,7 +5199,7 @@
       <c r="AF77" s="8"/>
       <c r="AG77" s="8"/>
     </row>
-    <row r="78" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A78" s="8"/>
       <c r="B78" s="8"/>
       <c r="C78" s="8"/>
@@ -5214,10 +5214,10 @@
       <c r="L78" s="8"/>
       <c r="M78" s="8"/>
       <c r="N78" s="3" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="O78" s="1" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="P78" s="12" t="s">
         <v>119</v>
@@ -5240,7 +5240,7 @@
       <c r="AF78" s="8"/>
       <c r="AG78" s="8"/>
     </row>
-    <row r="79" spans="1:36" ht="18" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:36" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A79" s="8"/>
       <c r="B79" s="8"/>
       <c r="C79" s="8"/>
@@ -5264,7 +5264,7 @@
         <v>121</v>
       </c>
       <c r="O79" s="1" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="P79" s="12" t="s">
         <v>120</v>
@@ -5290,7 +5290,7 @@
       <c r="AI79" s="8"/>
       <c r="AJ79" s="8"/>
     </row>
-    <row r="80" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A80" s="8"/>
       <c r="B80" s="8"/>
       <c r="C80" s="8"/>
@@ -5311,13 +5311,13 @@
       <c r="L80" s="8"/>
       <c r="M80" s="8"/>
       <c r="N80" s="3" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="O80" s="1" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="P80" s="12" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="Q80" s="8"/>
       <c r="R80" s="8"/>
@@ -5340,7 +5340,7 @@
       <c r="AI80" s="8"/>
       <c r="AJ80" s="8"/>
     </row>
-    <row r="81" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A81" s="8"/>
       <c r="B81" s="8"/>
       <c r="C81" s="8"/>
@@ -5361,13 +5361,13 @@
       <c r="L81" s="8"/>
       <c r="M81" s="8"/>
       <c r="N81" s="3" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="O81" s="1" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="P81" s="12" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="Q81" s="8"/>
       <c r="R81" s="8"/>
@@ -5390,7 +5390,7 @@
       <c r="AI81" s="8"/>
       <c r="AJ81" s="8"/>
     </row>
-    <row r="82" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A82" s="8"/>
       <c r="B82" s="8"/>
       <c r="C82" s="8"/>
@@ -5404,20 +5404,20 @@
         <v>107</v>
       </c>
       <c r="I82" s="12" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="J82" s="8"/>
       <c r="K82" s="8"/>
       <c r="L82" s="8"/>
       <c r="M82" s="8"/>
       <c r="N82" s="3" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="O82" s="1" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="P82" s="12" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="Q82" s="8"/>
       <c r="R82" s="8"/>
@@ -5440,7 +5440,7 @@
       <c r="AI82" s="8"/>
       <c r="AJ82" s="8"/>
     </row>
-    <row r="83" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A83" s="8"/>
       <c r="B83" s="8"/>
       <c r="C83" s="8"/>
@@ -5464,10 +5464,10 @@
         <v>54</v>
       </c>
       <c r="O83" s="1" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="P83" s="12" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="Q83" s="8"/>
       <c r="R83" s="8"/>
@@ -5490,7 +5490,7 @@
       <c r="AI83" s="8"/>
       <c r="AJ83" s="8"/>
     </row>
-    <row r="84" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A84" s="8"/>
       <c r="B84" s="8"/>
       <c r="C84" s="8"/>
@@ -5504,20 +5504,20 @@
         <v>113</v>
       </c>
       <c r="I84" s="12" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="J84" s="8"/>
       <c r="K84" s="8"/>
       <c r="L84" s="8"/>
       <c r="M84" s="8"/>
       <c r="N84" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="O84" s="1" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="P84" s="12" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="Q84" s="8"/>
       <c r="R84" s="8"/>
@@ -5540,7 +5540,7 @@
       <c r="AI84" s="8"/>
       <c r="AJ84" s="8"/>
     </row>
-    <row r="85" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A85" s="8"/>
       <c r="B85" s="8"/>
       <c r="C85" s="8"/>
@@ -5555,10 +5555,10 @@
       <c r="L85" s="8"/>
       <c r="M85" s="8"/>
       <c r="N85" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="O85" s="1" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="P85" s="12" t="s">
         <v>122</v>
@@ -5584,7 +5584,7 @@
       <c r="AI85" s="8"/>
       <c r="AJ85" s="8"/>
     </row>
-    <row r="86" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A86" s="8"/>
       <c r="B86" s="8"/>
       <c r="C86" s="8"/>
@@ -5599,10 +5599,10 @@
       <c r="L86" s="8"/>
       <c r="M86" s="8"/>
       <c r="N86" s="3" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="O86" s="1" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="P86" s="12" t="s">
         <v>138</v>
@@ -5628,7 +5628,7 @@
       <c r="AI86" s="8"/>
       <c r="AJ86" s="8"/>
     </row>
-    <row r="87" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A87" s="8"/>
       <c r="B87" s="8"/>
       <c r="C87" s="8"/>
@@ -5643,7 +5643,7 @@
       <c r="L87" s="8"/>
       <c r="M87" s="8"/>
       <c r="N87" s="3" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="O87" s="1" t="s">
         <v>28</v>
@@ -5672,7 +5672,7 @@
       <c r="AI87" s="8"/>
       <c r="AJ87" s="8"/>
     </row>
-    <row r="88" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A88" s="8"/>
       <c r="B88" s="8"/>
       <c r="C88" s="8"/>
@@ -5687,13 +5687,13 @@
       <c r="L88" s="8"/>
       <c r="M88" s="8"/>
       <c r="N88" s="3" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="O88" s="1" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="P88" s="12" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="Q88" s="8"/>
       <c r="R88" s="8"/>
@@ -5716,7 +5716,7 @@
       <c r="AI88" s="8"/>
       <c r="AJ88" s="8"/>
     </row>
-    <row r="89" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A89" s="8"/>
       <c r="B89" s="8"/>
       <c r="C89" s="8"/>
@@ -5731,7 +5731,7 @@
       <c r="L89" s="8"/>
       <c r="M89" s="8"/>
       <c r="N89" s="3" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="O89" s="1" t="s">
         <v>48</v>
@@ -5760,7 +5760,7 @@
       <c r="AI89" s="8"/>
       <c r="AJ89" s="8"/>
     </row>
-    <row r="90" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A90" s="8"/>
       <c r="B90" s="8"/>
       <c r="C90" s="8"/>
@@ -5775,13 +5775,13 @@
       <c r="L90" s="8"/>
       <c r="M90" s="8"/>
       <c r="N90" s="3" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="O90" s="1" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="P90" s="12" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="Q90" s="8"/>
       <c r="R90" s="8"/>
@@ -5804,7 +5804,7 @@
       <c r="AI90" s="8"/>
       <c r="AJ90" s="8"/>
     </row>
-    <row r="91" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A91" s="8"/>
       <c r="B91" s="8"/>
       <c r="C91" s="8"/>
@@ -5819,13 +5819,13 @@
       <c r="L91" s="8"/>
       <c r="M91" s="8"/>
       <c r="N91" s="3" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="O91" s="1" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="P91" s="12" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="Q91" s="8"/>
       <c r="R91" s="8"/>
@@ -5848,7 +5848,7 @@
       <c r="AI91" s="8"/>
       <c r="AJ91" s="8"/>
     </row>
-    <row r="92" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A92" s="8"/>
       <c r="B92" s="8"/>
       <c r="C92" s="8"/>
@@ -5863,13 +5863,13 @@
       <c r="L92" s="8"/>
       <c r="M92" s="8"/>
       <c r="N92" s="3" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="O92" s="1" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="P92" s="12" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="Q92" s="8"/>
       <c r="R92" s="8"/>
@@ -5892,7 +5892,7 @@
       <c r="AI92" s="8"/>
       <c r="AJ92" s="8"/>
     </row>
-    <row r="93" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A93" s="8"/>
       <c r="B93" s="8"/>
       <c r="C93" s="8"/>
@@ -5907,13 +5907,13 @@
       <c r="L93" s="8"/>
       <c r="M93" s="8"/>
       <c r="N93" s="3" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="O93" s="1" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="P93" s="12" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="Q93" s="8"/>
       <c r="R93" s="8"/>
@@ -5936,7 +5936,7 @@
       <c r="AI93" s="8"/>
       <c r="AJ93" s="8"/>
     </row>
-    <row r="94" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A94" s="8"/>
       <c r="B94" s="8"/>
       <c r="C94" s="8"/>
@@ -5951,7 +5951,7 @@
       <c r="L94" s="8"/>
       <c r="M94" s="8"/>
       <c r="N94" s="3" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="O94" s="1"/>
       <c r="P94" s="12" t="s">
@@ -5978,7 +5978,7 @@
       <c r="AI94" s="8"/>
       <c r="AJ94" s="8"/>
     </row>
-    <row r="95" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A95" s="8"/>
       <c r="B95" s="8"/>
       <c r="C95" s="8"/>
@@ -5993,7 +5993,7 @@
       <c r="L95" s="8"/>
       <c r="M95" s="8"/>
       <c r="N95" s="3" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="O95" s="1"/>
       <c r="P95" s="12" t="s">
@@ -6020,7 +6020,7 @@
       <c r="AI95" s="8"/>
       <c r="AJ95" s="8"/>
     </row>
-    <row r="96" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A96" s="8"/>
       <c r="B96" s="8"/>
       <c r="C96" s="8"/>
@@ -6062,7 +6062,7 @@
       <c r="AI96" s="8"/>
       <c r="AJ96" s="8"/>
     </row>
-    <row r="97" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A97" s="8"/>
       <c r="B97" s="8"/>
       <c r="C97" s="8"/>
@@ -6077,10 +6077,10 @@
       <c r="L97" s="8"/>
       <c r="M97" s="8"/>
       <c r="N97" s="3" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="O97" s="1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="P97" s="12" t="s">
         <v>57</v>
@@ -6106,7 +6106,7 @@
       <c r="AI97" s="8"/>
       <c r="AJ97" s="8"/>
     </row>
-    <row r="98" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A98" s="8"/>
       <c r="B98" s="8"/>
       <c r="C98" s="8"/>
@@ -6121,13 +6121,13 @@
       <c r="L98" s="8"/>
       <c r="M98" s="8"/>
       <c r="N98" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="O98" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="O98" s="1" t="s">
-        <v>323</v>
-      </c>
       <c r="P98" s="12" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="Q98" s="8"/>
       <c r="R98" s="8"/>
@@ -6150,7 +6150,7 @@
       <c r="AI98" s="8"/>
       <c r="AJ98" s="8"/>
     </row>
-    <row r="99" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A99" s="8"/>
       <c r="B99" s="8"/>
       <c r="C99" s="8"/>
@@ -6165,13 +6165,13 @@
       <c r="L99" s="8"/>
       <c r="M99" s="8"/>
       <c r="N99" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="O99" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="O99" s="1" t="s">
-        <v>324</v>
-      </c>
       <c r="P99" s="12" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="Q99" s="8"/>
       <c r="R99" s="8"/>
@@ -6194,7 +6194,7 @@
       <c r="AI99" s="8"/>
       <c r="AJ99" s="8"/>
     </row>
-    <row r="100" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A100" s="8"/>
       <c r="B100" s="8"/>
       <c r="C100" s="8"/>
@@ -6209,13 +6209,13 @@
       <c r="L100" s="8"/>
       <c r="M100" s="8"/>
       <c r="N100" s="3" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="O100" s="1" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="P100" s="12" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="Q100" s="8"/>
       <c r="R100" s="8"/>
@@ -6238,7 +6238,7 @@
       <c r="AI100" s="8"/>
       <c r="AJ100" s="8"/>
     </row>
-    <row r="101" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A101" s="8"/>
       <c r="B101" s="8"/>
       <c r="C101" s="8"/>
@@ -6253,13 +6253,13 @@
       <c r="L101" s="8"/>
       <c r="M101" s="8"/>
       <c r="N101" s="3" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="O101" s="1" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="P101" s="12" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="Q101" s="8"/>
       <c r="R101" s="8"/>
@@ -6282,7 +6282,7 @@
       <c r="AI101" s="8"/>
       <c r="AJ101" s="8"/>
     </row>
-    <row r="102" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A102" s="8"/>
       <c r="B102" s="8"/>
       <c r="C102" s="8"/>
@@ -6297,10 +6297,10 @@
       <c r="L102" s="8"/>
       <c r="M102" s="8"/>
       <c r="N102" s="3" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="O102" s="1" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="P102" s="12" t="s">
         <v>55</v>
@@ -6326,7 +6326,7 @@
       <c r="AI102" s="8"/>
       <c r="AJ102" s="8"/>
     </row>
-    <row r="103" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A103" s="8"/>
       <c r="B103" s="8"/>
       <c r="C103" s="8"/>
@@ -6341,10 +6341,10 @@
       <c r="L103" s="8"/>
       <c r="M103" s="8"/>
       <c r="N103" s="3" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="O103" s="1" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="P103" s="12" t="s">
         <v>56</v>
@@ -6370,7 +6370,7 @@
       <c r="AI103" s="8"/>
       <c r="AJ103" s="8"/>
     </row>
-    <row r="104" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A104" s="8"/>
       <c r="B104" s="8"/>
       <c r="C104" s="8"/>
@@ -6408,7 +6408,7 @@
       <c r="AI104" s="8"/>
       <c r="AJ104" s="8"/>
     </row>
-    <row r="105" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A105" s="8"/>
       <c r="B105" s="8"/>
       <c r="C105" s="8"/>
@@ -6446,7 +6446,7 @@
       <c r="AI105" s="8"/>
       <c r="AJ105" s="8"/>
     </row>
-    <row r="106" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A106" s="8"/>
       <c r="B106" s="8"/>
       <c r="C106" s="8"/>
@@ -6461,13 +6461,13 @@
       <c r="L106" s="8"/>
       <c r="M106" s="8"/>
       <c r="N106" s="3" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="O106" s="1" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="P106" s="12" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="Q106" s="8"/>
       <c r="R106" s="8"/>
@@ -6490,7 +6490,7 @@
       <c r="AI106" s="8"/>
       <c r="AJ106" s="8"/>
     </row>
-    <row r="107" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A107" s="8"/>
       <c r="B107" s="8"/>
       <c r="C107" s="8"/>
@@ -6505,13 +6505,13 @@
       <c r="L107" s="8"/>
       <c r="M107" s="8"/>
       <c r="N107" s="3" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="O107" s="1" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="P107" s="12" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="Q107" s="8"/>
       <c r="R107" s="8"/>
@@ -6534,7 +6534,7 @@
       <c r="AI107" s="8"/>
       <c r="AJ107" s="8"/>
     </row>
-    <row r="108" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A108" s="8"/>
       <c r="B108" s="8"/>
       <c r="C108" s="8"/>
@@ -6549,13 +6549,13 @@
       <c r="L108" s="8"/>
       <c r="M108" s="8"/>
       <c r="N108" s="3" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="O108" s="1" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="P108" s="12" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="Q108" s="8"/>
       <c r="R108" s="8"/>
@@ -6575,7 +6575,7 @@
       <c r="AF108" s="8"/>
       <c r="AG108" s="8"/>
     </row>
-    <row r="109" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A109" s="8"/>
       <c r="B109" s="8"/>
       <c r="C109" s="8"/>
@@ -6590,13 +6590,13 @@
       <c r="L109" s="8"/>
       <c r="M109" s="8"/>
       <c r="N109" s="3" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="O109" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="P109" s="12" t="s">
         <v>349</v>
-      </c>
-      <c r="P109" s="12" t="s">
-        <v>353</v>
       </c>
       <c r="Q109" s="8"/>
       <c r="R109" s="8"/>
@@ -6616,7 +6616,7 @@
       <c r="AF109" s="8"/>
       <c r="AG109" s="8"/>
     </row>
-    <row r="110" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A110" s="8"/>
       <c r="B110" s="8"/>
       <c r="C110" s="8"/>
@@ -6631,11 +6631,11 @@
       <c r="L110" s="8"/>
       <c r="M110" s="8"/>
       <c r="N110" s="3" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="O110" s="1"/>
       <c r="P110" s="12" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="Q110" s="8"/>
       <c r="R110" s="8"/>
@@ -6655,7 +6655,7 @@
       <c r="AF110" s="8"/>
       <c r="AG110" s="8"/>
     </row>
-    <row r="111" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A111" s="8"/>
       <c r="B111" s="8"/>
       <c r="C111" s="8"/>
@@ -6670,13 +6670,13 @@
       <c r="L111" s="8"/>
       <c r="M111" s="8"/>
       <c r="N111" s="3" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="O111" s="1" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="P111" s="12" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="Q111" s="8"/>
       <c r="R111" s="8"/>
@@ -6696,7 +6696,7 @@
       <c r="AF111" s="8"/>
       <c r="AG111" s="8"/>
     </row>
-    <row r="112" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A112" s="8"/>
       <c r="B112" s="8"/>
       <c r="C112" s="8"/>
@@ -6711,11 +6711,11 @@
       <c r="L112" s="8"/>
       <c r="M112" s="8"/>
       <c r="N112" s="3" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="O112" s="1"/>
       <c r="P112" s="12" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="Q112" s="8"/>
       <c r="R112" s="8"/>
@@ -6738,7 +6738,7 @@
       <c r="AI112" s="8"/>
       <c r="AJ112" s="8"/>
     </row>
-    <row r="113" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A113" s="8"/>
       <c r="B113" s="8"/>
       <c r="C113" s="8"/>
@@ -6753,13 +6753,13 @@
       <c r="L113" s="8"/>
       <c r="M113" s="8"/>
       <c r="N113" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="O113" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="O113" s="1" t="s">
-        <v>351</v>
-      </c>
       <c r="P113" s="12" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="Q113" s="8"/>
       <c r="R113" s="8"/>
@@ -6782,7 +6782,7 @@
       <c r="AI113" s="8"/>
       <c r="AJ113" s="8"/>
     </row>
-    <row r="114" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A114" s="8"/>
       <c r="B114" s="8"/>
       <c r="C114" s="8"/>
@@ -6797,11 +6797,11 @@
       <c r="L114" s="8"/>
       <c r="M114" s="8"/>
       <c r="N114" s="3" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="O114" s="1"/>
       <c r="P114" s="12" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="Q114" s="8"/>
       <c r="R114" s="8"/>
@@ -6824,7 +6824,7 @@
       <c r="AI114" s="8"/>
       <c r="AJ114" s="8"/>
     </row>
-    <row r="115" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A115" s="8"/>
       <c r="B115" s="8"/>
       <c r="C115" s="8"/>
@@ -6839,13 +6839,13 @@
       <c r="L115" s="8"/>
       <c r="M115" s="8"/>
       <c r="N115" s="3" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="O115" s="1" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="P115" s="12" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="Q115" s="8"/>
       <c r="R115" s="8"/>
@@ -6868,7 +6868,7 @@
       <c r="AI115" s="8"/>
       <c r="AJ115" s="8"/>
     </row>
-    <row r="116" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A116" s="8"/>
       <c r="B116" s="8"/>
       <c r="C116" s="8"/>
@@ -6906,17 +6906,17 @@
       <c r="AI116" s="8"/>
       <c r="AJ116" s="8"/>
     </row>
-    <row r="117" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:36" x14ac:dyDescent="0.25">
       <c r="N117" s="3"/>
       <c r="O117" s="1"/>
       <c r="P117" s="12"/>
     </row>
-    <row r="118" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:36" x14ac:dyDescent="0.25">
       <c r="N118" s="3"/>
       <c r="O118" s="1"/>
       <c r="P118" s="12"/>
     </row>
-    <row r="119" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:36" x14ac:dyDescent="0.25">
       <c r="N119" s="3"/>
       <c r="O119" s="1"/>
       <c r="P119" s="12"/>
@@ -6942,15 +6942,15 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="39.88671875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="40.5546875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="52.44140625" customWidth="1"/>
+    <col min="1" max="1" width="33.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="39.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="40.5703125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="52.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="23.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -6964,42 +6964,42 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>30</v>
       </c>
@@ -7007,7 +7007,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>32</v>
       </c>
@@ -7015,97 +7015,97 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D47" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D48" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D49" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D50" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D51" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D52" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D54" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D55" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D56" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D57" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D58" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D59" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D60" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D61" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D62" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D63" t="s">
         <v>6</v>
       </c>
@@ -7113,12 +7113,12 @@
         <v>102</v>
       </c>
     </row>
-    <row r="64" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D64" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B78" s="2" t="s">
         <v>127</v>
       </c>
@@ -7126,7 +7126,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B79" s="2" t="s">
         <v>127</v>
       </c>
@@ -7134,7 +7134,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B80" s="2" t="s">
         <v>132</v>
       </c>
@@ -7142,7 +7142,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B81" s="2" t="s">
         <v>131</v>
       </c>

</xml_diff>